<commit_message>
swapped colors and markers, updated excel
</commit_message>
<xml_diff>
--- a/clusters/cl_neg_with_std.xlsx
+++ b/clusters/cl_neg_with_std.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\slu\projects\project\clusters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C85186-98A2-49D6-A767-2D9BEC9D44E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5009567C-0295-4556-A346-9FC76B9CDC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,42 +37,12 @@
     <t>model</t>
   </si>
   <si>
-    <t>statement neg</t>
-  </si>
-  <si>
-    <t>cooperation neg</t>
-  </si>
-  <si>
-    <t>retreat neg</t>
-  </si>
-  <si>
-    <t>investigation neg</t>
-  </si>
-  <si>
     <t>demand neg</t>
   </si>
   <si>
-    <t>dissaproval neg</t>
-  </si>
-  <si>
-    <t>rejection neg</t>
-  </si>
-  <si>
-    <t>threat neg</t>
-  </si>
-  <si>
     <t>protest neg</t>
   </si>
   <si>
-    <t>force neg</t>
-  </si>
-  <si>
-    <t>relation neg</t>
-  </si>
-  <si>
-    <t>coercion neg</t>
-  </si>
-  <si>
     <t>assault neg</t>
   </si>
   <si>
@@ -94,7 +64,37 @@
     <t>vanilla-gpt-4</t>
   </si>
   <si>
-    <t>hybrid attack neg</t>
+    <t>make statement neg</t>
+  </si>
+  <si>
+    <t>cooperate neg</t>
+  </si>
+  <si>
+    <t>yield neg</t>
+  </si>
+  <si>
+    <t>investigate neg</t>
+  </si>
+  <si>
+    <t>disapprove neg</t>
+  </si>
+  <si>
+    <t>reject neg</t>
+  </si>
+  <si>
+    <t>threaten neg</t>
+  </si>
+  <si>
+    <t>exhibit force neg</t>
+  </si>
+  <si>
+    <t>reduce relations neg</t>
+  </si>
+  <si>
+    <t>coerce neg</t>
+  </si>
+  <si>
+    <t>mass violence neg</t>
   </si>
 </sst>
 </file>
@@ -464,13 +464,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="L62" sqref="L62"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -501,10 +501,10 @@
         <v>8.1989159174992299</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -518,10 +518,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -535,10 +535,10 @@
         <v>5.5277079839256666</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -552,10 +552,10 @@
         <v>15.45603082582617</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -569,10 +569,10 @@
         <v>7.4535599249992988</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -586,10 +586,10 @@
         <v>3.771236166328253</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -603,10 +603,10 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -620,10 +620,10 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -637,10 +637,10 @@
         <v>27.688746209726919</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -654,10 +654,10 @@
         <v>6.8718427093627676</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -671,10 +671,10 @@
         <v>24.299634199350042</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -688,10 +688,10 @@
         <v>18.63389981249825</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -705,10 +705,10 @@
         <v>6.8718427093627676</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -722,10 +722,10 @@
         <v>38.014982426523481</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -739,10 +739,10 @@
         <v>6.8718427093627676</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -756,10 +756,10 @@
         <v>5.7735026918962582</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -773,10 +773,10 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -790,10 +790,10 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -807,10 +807,10 @@
         <v>19.238993967691989</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -824,10 +824,10 @@
         <v>6.8718427093627676</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -841,10 +841,10 @@
         <v>6.5996632910744433</v>
       </c>
       <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
         <v>9</v>
-      </c>
-      <c r="E22" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -858,10 +858,10 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -875,10 +875,10 @@
         <v>11.08329852403334</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -892,10 +892,10 @@
         <v>24.355900240869971</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -909,10 +909,10 @@
         <v>6.8493488921877521</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -926,10 +926,10 @@
         <v>2.8867513459481291</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E27" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -943,10 +943,10 @@
         <v>18.63389981249825</v>
       </c>
       <c r="D28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" t="s">
         <v>10</v>
-      </c>
-      <c r="E28" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -960,10 +960,10 @@
         <v>5.7735026918962582</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E29" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -977,10 +977,10 @@
         <v>24.438130497691969</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E30" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -994,10 +994,10 @@
         <v>7.6376261582597333</v>
       </c>
       <c r="D31" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E31" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1011,10 +1011,10 @@
         <v>5.217491947499509</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E32" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1028,10 +1028,10 @@
         <v>18.63389981249825</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E33" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1045,10 +1045,10 @@
         <v>5.3359368645273726</v>
       </c>
       <c r="D34" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" t="s">
         <v>11</v>
-      </c>
-      <c r="E34" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1062,10 +1062,10 @@
         <v>23.570226039551589</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E35" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1079,10 +1079,10 @@
         <v>3.7267799624996489</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E36" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1096,10 +1096,10 @@
         <v>10.17212967977809</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E37" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1113,10 +1113,10 @@
         <v>19.720265943665389</v>
       </c>
       <c r="D38" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E38" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1130,10 +1130,10 @@
         <v>3.7267799624996489</v>
       </c>
       <c r="D39" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E39" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1147,10 +1147,10 @@
         <v>35.433819375782157</v>
       </c>
       <c r="D40" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" t="s">
         <v>12</v>
-      </c>
-      <c r="E40" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1164,10 +1164,10 @@
         <v>7.4535599249992988</v>
       </c>
       <c r="D41" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E41" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1181,10 +1181,10 @@
         <v>13.801167422440111</v>
       </c>
       <c r="D42" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E42" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1198,10 +1198,10 @@
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1215,10 +1215,10 @@
         <v>6.7185481235821243</v>
       </c>
       <c r="D44" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E44" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1232,10 +1232,10 @@
         <v>33.96280645385805</v>
       </c>
       <c r="D45" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E45" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1249,10 +1249,10 @@
         <v>4.714045207910317</v>
       </c>
       <c r="D46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
         <v>13</v>
-      </c>
-      <c r="E46" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1266,10 +1266,10 @@
         <v>5.0332229568471663</v>
       </c>
       <c r="D47" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E47" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1283,10 +1283,10 @@
         <v>18.63389981249825</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E48" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1300,10 +1300,10 @@
         <v>6.0667582410670988</v>
       </c>
       <c r="D49" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E49" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1317,10 +1317,10 @@
         <v>21.14762923408253</v>
       </c>
       <c r="D50" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E50" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1334,10 +1334,10 @@
         <v>7.6376261582597333</v>
       </c>
       <c r="D51" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E51" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1351,10 +1351,10 @@
         <v>8.2272413359521668</v>
       </c>
       <c r="D52" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E52" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1368,10 +1368,10 @@
         <v>21.650635094610969</v>
       </c>
       <c r="D53" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E53" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1385,10 +1385,10 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E54" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1402,10 +1402,10 @@
         <v>28.36701429477554</v>
       </c>
       <c r="D55" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E55" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1419,10 +1419,10 @@
         <v>4.3301270189221936</v>
       </c>
       <c r="D56" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E56" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1436,10 +1436,10 @@
         <v>7</v>
       </c>
       <c r="D57" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E57" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1453,10 +1453,10 @@
         <v>21.650635094610969</v>
       </c>
       <c r="D58" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E58" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1470,10 +1470,10 @@
         <v>6.9597054535375271</v>
       </c>
       <c r="D59" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E59" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1487,10 +1487,10 @@
         <v>27.034410942352711</v>
       </c>
       <c r="D60" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E60" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1504,10 +1504,10 @@
         <v>6.6143782776614763</v>
       </c>
       <c r="D61" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E61" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1521,10 +1521,10 @@
         <v>6.9530332375024688</v>
       </c>
       <c r="D62" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E62" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1538,10 +1538,10 @@
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E63" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1555,10 +1555,10 @@
         <v>4.9943278484292932</v>
       </c>
       <c r="D64" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E64" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1572,10 +1572,10 @@
         <v>19.06249419166485</v>
       </c>
       <c r="D65" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E65" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1589,10 +1589,10 @@
         <v>7.737179432986629</v>
       </c>
       <c r="D66" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E66" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1606,10 +1606,10 @@
         <v>7.2076776623230474</v>
       </c>
       <c r="D67" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E67" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1623,10 +1623,10 @@
         <v>23.094010767585029</v>
       </c>
       <c r="D68" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E68" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1640,10 +1640,10 @@
         <v>6.2853936105470893</v>
       </c>
       <c r="D69" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E69" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1657,10 +1657,10 @@
         <v>24.279748203791289</v>
       </c>
       <c r="D70" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E70" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -1674,10 +1674,10 @@
         <v>8.7488976377909022</v>
       </c>
       <c r="D71" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E71" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1694,7 +1694,7 @@
         <v>24</v>
       </c>
       <c r="E72" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1711,7 +1711,7 @@
         <v>24</v>
       </c>
       <c r="E73" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1728,7 +1728,7 @@
         <v>24</v>
       </c>
       <c r="E74" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -1745,7 +1745,7 @@
         <v>24</v>
       </c>
       <c r="E75" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -1762,7 +1762,7 @@
         <v>24</v>
       </c>
       <c r="E76" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>